<commit_message>
Collar hitboxes, recipe tweaks
</commit_message>
<xml_diff>
--- a/Outline.xlsx
+++ b/Outline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ECO\Modding\VEcoMods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC09B1F4-5056-4FB2-8C0F-7A8B2BCB575E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8467D73-337D-4FB2-8B32-745BA988DAC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="10440" activeTab="2" xr2:uid="{A33CFE89-0774-4CFB-8D60-F9AFB2F57947}"/>
   </bookViews>
@@ -2781,16 +2781,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2805,7 +2805,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17145000" y="381000"/>
+          <a:off x="7734300" y="6143625"/>
           <a:ext cx="1143000" cy="571499"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -2851,16 +2851,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2875,8 +2875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14906625" y="1285876"/>
-          <a:ext cx="1152525" cy="371474"/>
+          <a:off x="5743575" y="6858001"/>
+          <a:ext cx="1047750" cy="409574"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2921,16 +2921,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2945,8 +2945,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18183225" y="1314451"/>
-          <a:ext cx="1028700" cy="361950"/>
+          <a:off x="7553325" y="6886576"/>
+          <a:ext cx="1028700" cy="390524"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -2991,16 +2991,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3015,8 +3015,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14982825" y="2476500"/>
-          <a:ext cx="1123950" cy="514349"/>
+          <a:off x="5724525" y="8124825"/>
+          <a:ext cx="1019175" cy="514349"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3061,16 +3061,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3914775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3085,8 +3085,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14297025" y="1314451"/>
-          <a:ext cx="1019175" cy="361950"/>
+          <a:off x="3914775" y="6886575"/>
+          <a:ext cx="1019175" cy="304799"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3131,16 +3131,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2800349</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3629024</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3155,8 +3155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13182599" y="2133600"/>
-          <a:ext cx="828675" cy="485775"/>
+          <a:off x="2800349" y="7515225"/>
+          <a:ext cx="828675" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3201,16 +3201,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2600325</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3225,8 +3225,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10972800" y="2133601"/>
-          <a:ext cx="790575" cy="361950"/>
+          <a:off x="1809750" y="7515225"/>
+          <a:ext cx="790575" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3271,16 +3271,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2457450</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3248025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3295,7 +3295,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11620500" y="400051"/>
+          <a:off x="2457450" y="6162676"/>
           <a:ext cx="790575" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -3341,16 +3341,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19052</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3365,7 +3365,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14239875" y="209552"/>
+          <a:off x="5076825" y="5972177"/>
           <a:ext cx="1285875" cy="276224"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -3411,16 +3411,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180977</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3435,8 +3435,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15697200" y="180977"/>
-          <a:ext cx="962025" cy="314324"/>
+          <a:off x="6429375" y="5943602"/>
+          <a:ext cx="819150" cy="314324"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3481,16 +3481,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3505,7 +3505,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12925425" y="447676"/>
+          <a:off x="3762375" y="6210301"/>
           <a:ext cx="1019175" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -3551,16 +3551,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>461963</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>442913</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3578,8 +3578,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14882813" y="485776"/>
-          <a:ext cx="600075" cy="800100"/>
+          <a:off x="5719763" y="6248401"/>
+          <a:ext cx="547687" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3607,16 +3607,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>538163</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3634,8 +3634,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="15482888" y="495301"/>
-          <a:ext cx="695325" cy="790575"/>
+          <a:off x="6267450" y="6257926"/>
+          <a:ext cx="571500" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3663,16 +3663,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3690,8 +3690,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="18697575" y="952499"/>
-          <a:ext cx="238125" cy="361952"/>
+          <a:off x="8067675" y="6715124"/>
+          <a:ext cx="238125" cy="171452"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3719,16 +3719,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>452438</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>347663</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3745,9 +3745,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15482888" y="1657350"/>
-          <a:ext cx="61912" cy="819150"/>
+        <a:xfrm flipH="1">
+          <a:off x="6234113" y="7267575"/>
+          <a:ext cx="33337" cy="857250"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3775,16 +3775,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>233363</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>385763</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3802,8 +3802,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14654213" y="809626"/>
-          <a:ext cx="152400" cy="504825"/>
+          <a:off x="4271963" y="6572251"/>
+          <a:ext cx="152400" cy="314324"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3831,16 +3831,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2852738</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3214687</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3858,8 +3858,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="12730163" y="1266825"/>
-          <a:ext cx="1371599" cy="361949"/>
+          <a:off x="2538413" y="6838950"/>
+          <a:ext cx="990599" cy="361949"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -3887,16 +3887,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>604838</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2205039</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2852739</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3914,8 +3914,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="11006138" y="1123951"/>
-          <a:ext cx="1371600" cy="647700"/>
+          <a:off x="2033589" y="6696075"/>
+          <a:ext cx="990599" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -3943,16 +3943,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>352425</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2852738</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3914775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3970,8 +3970,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="13399294" y="597694"/>
-          <a:ext cx="733425" cy="1062037"/>
+          <a:off x="3126582" y="6250781"/>
+          <a:ext cx="514349" cy="1062037"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -3999,16 +3999,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1724025</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4023,8 +4023,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11239500" y="2057401"/>
-          <a:ext cx="866775" cy="466724"/>
+          <a:off x="685800" y="7439026"/>
+          <a:ext cx="1038225" cy="276224"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4069,16 +4069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>300038</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1204913</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2852738</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4096,8 +4096,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="11806238" y="628651"/>
-          <a:ext cx="1295400" cy="1562100"/>
+          <a:off x="1571626" y="6157914"/>
+          <a:ext cx="914400" cy="1647825"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4125,16 +4125,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3438524</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4149,7 +4149,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13820774" y="3257550"/>
+          <a:off x="3438524" y="8448675"/>
           <a:ext cx="828675" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -4195,16 +4195,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4219,7 +4219,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18459449" y="3076575"/>
+          <a:off x="7858124" y="8658225"/>
           <a:ext cx="1314451" cy="742950"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -4278,16 +4278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>238124</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4302,7 +4302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15049499" y="3162300"/>
+          <a:off x="4724399" y="8743950"/>
           <a:ext cx="828675" cy="485775"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
@@ -4348,16 +4348,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>423862</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3214686</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3852861</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4375,8 +4375,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="13596937" y="2619374"/>
-          <a:ext cx="638175" cy="638175"/>
+          <a:off x="3305174" y="7900987"/>
+          <a:ext cx="457200" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4404,16 +4404,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>423863</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3852863</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4431,8 +4431,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="14235113" y="2733674"/>
-          <a:ext cx="1966913" cy="523875"/>
+          <a:off x="3852863" y="8381999"/>
+          <a:ext cx="1871663" cy="66675"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -4460,16 +4460,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>423863</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>385764</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3852863</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>366714</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4487,8 +4487,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="13730289" y="2181225"/>
-          <a:ext cx="1581149" cy="571501"/>
+          <a:off x="3509963" y="7534274"/>
+          <a:ext cx="1257301" cy="571501"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4516,16 +4516,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>433386</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2205037</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>471486</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4543,12 +4543,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="13449300" y="1633538"/>
-          <a:ext cx="1152524" cy="2876549"/>
+          <a:off x="3052762" y="7143750"/>
+          <a:ext cx="1238250" cy="2933699"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 119835"/>
+            <a:gd name="adj1" fmla="val 118462"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4574,16 +4574,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28576</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>471488</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>347664</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4601,12 +4601,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="15785306" y="2669381"/>
-          <a:ext cx="657226" cy="1300163"/>
+          <a:off x="5391150" y="8386761"/>
+          <a:ext cx="590551" cy="1095376"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 134783"/>
+            <a:gd name="adj1" fmla="val 138710"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -4632,16 +4632,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4656,8 +4656,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16935449" y="3209924"/>
-          <a:ext cx="1171575" cy="561975"/>
+          <a:off x="6429374" y="8839199"/>
+          <a:ext cx="1028700" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4702,16 +4702,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>328613</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>280988</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3629024</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4729,8 +4729,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="14011274" y="1471613"/>
-          <a:ext cx="2114551" cy="904875"/>
+          <a:off x="3629024" y="7062788"/>
+          <a:ext cx="2114551" cy="690562"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4758,16 +4758,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4785,8 +4785,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17325975" y="2733675"/>
-          <a:ext cx="195262" cy="476249"/>
+          <a:off x="6743700" y="8382000"/>
+          <a:ext cx="200024" cy="457199"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -4814,16 +4814,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>385763</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142873</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4841,8 +4841,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="16261557" y="221457"/>
-          <a:ext cx="1400174" cy="4310062"/>
+          <a:off x="5736431" y="5879305"/>
+          <a:ext cx="1466851" cy="4090987"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4870,16 +4870,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4897,8 +4897,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17325975" y="2733675"/>
-          <a:ext cx="1790700" cy="342900"/>
+          <a:off x="6743700" y="8382000"/>
+          <a:ext cx="1771650" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -4926,16 +4926,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4953,8 +4953,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="18207038" y="2166938"/>
-          <a:ext cx="1400174" cy="419100"/>
+          <a:off x="7600950" y="7743824"/>
+          <a:ext cx="1381125" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4982,16 +4982,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5006,8 +5006,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19935825" y="666750"/>
-          <a:ext cx="1143000" cy="571499"/>
+          <a:off x="9305925" y="6429375"/>
+          <a:ext cx="1143000" cy="380999"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5052,16 +5052,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>423863</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3852863</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>352426</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5079,12 +5079,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="15675770" y="235744"/>
-          <a:ext cx="1581149" cy="4462463"/>
+          <a:off x="5374482" y="5755481"/>
+          <a:ext cx="1171575" cy="4214813"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 30121"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -5110,16 +5110,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>328613</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>352426</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5137,8 +5137,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17278350" y="1471613"/>
-          <a:ext cx="904875" cy="23813"/>
+          <a:off x="6791325" y="7062788"/>
+          <a:ext cx="762000" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5167,16 +5167,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>352426</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -5194,8 +5194,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="18678525" y="952500"/>
-          <a:ext cx="723900" cy="542926"/>
+          <a:off x="8582025" y="6619875"/>
+          <a:ext cx="723900" cy="461963"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -15132,10 +15132,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34755E8F-0762-44A5-867E-91DAB55A1407}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15147,65 +15147,68 @@
     <col min="24" max="24" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
       <c r="D1" t="s">
         <v>95</v>
       </c>
-      <c r="Q1" t="s">
-        <v>99</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
some changes made hile attempting rubble
</commit_message>
<xml_diff>
--- a/Outline.xlsx
+++ b/Outline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ECO\Modding\VEcoMods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8467D73-337D-4FB2-8B32-745BA988DAC6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5257D70B-66F4-446B-B0BD-AA3CEE157D51}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="10440" activeTab="2" xr2:uid="{A33CFE89-0774-4CFB-8D60-F9AFB2F57947}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="10440" activeTab="1" xr2:uid="{A33CFE89-0774-4CFB-8D60-F9AFB2F57947}"/>
   </bookViews>
   <sheets>
     <sheet name="Advanced Mining" sheetId="1" r:id="rId1"/>
@@ -473,9 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -489,6 +486,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14461,21 +14461,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -14681,8 +14681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F82F47F-3B1D-413C-9837-C27255EC7E5B}">
   <dimension ref="A2:T41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14834,11 +14834,11 @@
         <v>10</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28:O28" si="0">N26*M28</f>
+        <f>N26*M28</f>
         <v>5</v>
       </c>
       <c r="O28">
-        <f t="shared" si="0"/>
+        <f>O26*N28</f>
         <v>4</v>
       </c>
       <c r="P28">
@@ -14998,7 +14998,7 @@
         <v>74</v>
       </c>
       <c r="M36">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N36">
         <v>0.5</v>
@@ -15038,20 +15038,19 @@
         <v>10</v>
       </c>
       <c r="M38">
-        <f>M36*L38</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N38">
-        <f t="shared" ref="N38:O38" si="1">N36*M38</f>
-        <v>5</v>
+        <f>N36*M38</f>
+        <v>6</v>
       </c>
       <c r="O38">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>O36*N38</f>
+        <v>3.5999999999999996</v>
       </c>
       <c r="P38">
         <f>P36*M38</f>
-        <v>3</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="Q38">
         <f>Q36*L38</f>
@@ -15059,7 +15058,7 @@
       </c>
       <c r="R38">
         <f>1/((L38*30)/(O38*4))</f>
-        <v>0.04</v>
+        <v>4.7999999999999994E-2</v>
       </c>
     </row>
     <row r="39" spans="3:18" x14ac:dyDescent="0.25">
@@ -15068,19 +15067,19 @@
       </c>
       <c r="M39">
         <f>M36*L39/$M24</f>
-        <v>14.285714285714286</v>
+        <v>17.142857142857142</v>
       </c>
       <c r="N39">
         <f>N36*M39/$M24</f>
-        <v>10.204081632653063</v>
+        <v>12.244897959183675</v>
       </c>
       <c r="O39">
         <f>O36*N39/$N24</f>
-        <v>30.612244897959187</v>
+        <v>36.734693877551017</v>
       </c>
       <c r="P39">
         <f>P36*M39/$N24</f>
-        <v>21.428571428571427</v>
+        <v>25.714285714285712</v>
       </c>
       <c r="Q39">
         <f>Q36*L39/0.2</f>
@@ -15088,7 +15087,7 @@
       </c>
       <c r="R39">
         <f>1/((L39*30)/(O39*4))</f>
-        <v>0.40816326530612251</v>
+        <v>0.48979591836734687</v>
       </c>
     </row>
     <row r="40" spans="3:18" x14ac:dyDescent="0.25">
@@ -15097,11 +15096,11 @@
       </c>
       <c r="N40">
         <f>N35*N38</f>
-        <v>8</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="P40">
         <f>P35*P38</f>
-        <v>4.8000000000000007</v>
+        <v>5.76</v>
       </c>
       <c r="Q40">
         <f>Q35*Q38</f>
@@ -15114,11 +15113,11 @@
       </c>
       <c r="N41">
         <f>N35*N39</f>
-        <v>16.326530612244902</v>
+        <v>19.591836734693882</v>
       </c>
       <c r="P41">
         <f>P35*P39</f>
-        <v>34.285714285714285</v>
+        <v>41.142857142857139</v>
       </c>
       <c r="Q41">
         <f>Q35*Q39</f>
@@ -15134,8 +15133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34755E8F-0762-44A5-867E-91DAB55A1407}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15156,47 +15155,47 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -15232,7 +15231,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>98</v>
       </c>
     </row>
@@ -15263,283 +15262,283 @@
     <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="13:23" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="7" t="s">
+      <c r="M33" s="4"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="8"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="7"/>
     </row>
     <row r="34" spans="13:23" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M34" s="9"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="11"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="10"/>
     </row>
     <row r="35" spans="13:23" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M35" s="9"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="11"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="10"/>
     </row>
     <row r="36" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M36" s="9"/>
-      <c r="N36" s="10"/>
-      <c r="O36" s="10"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="10"/>
-      <c r="R36" s="10"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
-      <c r="W36" s="11"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="10"/>
     </row>
     <row r="37" spans="13:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M37" s="9"/>
-      <c r="N37" s="10"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
-      <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
-      <c r="W37" s="11"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="10"/>
     </row>
     <row r="38" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M38" s="9"/>
-      <c r="N38" s="10"/>
-      <c r="O38" s="10"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="10"/>
-      <c r="R38" s="10"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
-      <c r="W38" s="11"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="10"/>
     </row>
     <row r="39" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M39" s="9"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
-      <c r="W39" s="11"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="10"/>
     </row>
     <row r="40" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M40" s="9"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
-      <c r="W40" s="11"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="10"/>
     </row>
     <row r="41" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M41" s="9"/>
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
-      <c r="W41" s="11"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="10"/>
     </row>
     <row r="42" spans="13:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M42" s="9"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
-      <c r="U42" s="10"/>
-      <c r="V42" s="10"/>
-      <c r="W42" s="11"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="10"/>
     </row>
     <row r="43" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M43" s="9"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
-      <c r="W43" s="11"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="10"/>
     </row>
     <row r="44" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M44" s="9"/>
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-      <c r="S44" s="10"/>
-      <c r="T44" s="10"/>
-      <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
-      <c r="W44" s="11"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="10"/>
     </row>
     <row r="45" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M45" s="9"/>
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-      <c r="S45" s="10"/>
-      <c r="T45" s="10"/>
-      <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
-      <c r="W45" s="11"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="9"/>
+      <c r="V45" s="9"/>
+      <c r="W45" s="10"/>
     </row>
     <row r="46" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M46" s="9"/>
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
-      <c r="W46" s="11"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="10"/>
     </row>
     <row r="47" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M47" s="9"/>
-      <c r="N47" s="10"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="10"/>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="S47" s="10"/>
-      <c r="T47" s="10"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
-      <c r="W47" s="11"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="10"/>
     </row>
     <row r="48" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M48" s="9"/>
-      <c r="N48" s="10"/>
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-      <c r="S48" s="10"/>
-      <c r="T48" s="10"/>
-      <c r="U48" s="10"/>
-      <c r="V48" s="10"/>
-      <c r="W48" s="11"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="10"/>
     </row>
     <row r="49" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M49" s="9"/>
-      <c r="N49" s="10"/>
-      <c r="O49" s="10"/>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="10"/>
-      <c r="R49" s="10"/>
-      <c r="S49" s="10"/>
-      <c r="T49" s="10"/>
-      <c r="U49" s="10"/>
-      <c r="V49" s="10"/>
-      <c r="W49" s="11"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+      <c r="V49" s="9"/>
+      <c r="W49" s="10"/>
     </row>
     <row r="50" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M50" s="9"/>
-      <c r="N50" s="10"/>
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-      <c r="Q50" s="10"/>
-      <c r="R50" s="10"/>
-      <c r="S50" s="10"/>
-      <c r="T50" s="10"/>
-      <c r="U50" s="10"/>
-      <c r="V50" s="10"/>
-      <c r="W50" s="11"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="9"/>
+      <c r="U50" s="9"/>
+      <c r="V50" s="9"/>
+      <c r="W50" s="10"/>
     </row>
     <row r="51" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M51" s="9"/>
-      <c r="N51" s="10"/>
-      <c r="O51" s="10"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="10"/>
-      <c r="R51" s="10"/>
-      <c r="S51" s="10"/>
-      <c r="T51" s="10"/>
-      <c r="U51" s="10"/>
-      <c r="V51" s="10"/>
-      <c r="W51" s="11"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="10"/>
     </row>
     <row r="52" spans="13:23" x14ac:dyDescent="0.25">
-      <c r="M52" s="9"/>
-      <c r="N52" s="10"/>
-      <c r="O52" s="10"/>
-      <c r="P52" s="10"/>
-      <c r="Q52" s="10"/>
-      <c r="R52" s="10"/>
-      <c r="S52" s="10"/>
-      <c r="T52" s="10"/>
-      <c r="U52" s="10"/>
-      <c r="V52" s="10"/>
-      <c r="W52" s="11"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="9"/>
+      <c r="T52" s="9"/>
+      <c r="U52" s="9"/>
+      <c r="V52" s="9"/>
+      <c r="W52" s="10"/>
     </row>
     <row r="53" spans="13:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M53" s="12"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="13"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="13"/>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="13"/>
-      <c r="V53" s="13"/>
-      <c r="W53" s="14"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="12"/>
+      <c r="U53" s="12"/>
+      <c r="V53" s="12"/>
+      <c r="W53" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="68" scale="88" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="68" scale="57" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>